<commit_message>
more work on updated Rev B schematic/pcb
</commit_message>
<xml_diff>
--- a/kicad/BOM-revB.xlsx
+++ b/kicad/BOM-revB.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9961BF72-44C0-4E1B-8821-F155B6E77079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8565D0-7917-40D5-85B8-20269F72148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42540" yWindow="2775" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="32400" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-revB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -100,9 +100,6 @@
     <t xml:space="preserve">J1, </t>
   </si>
   <si>
-    <t>USB_B_Mini</t>
-  </si>
-  <si>
     <t xml:space="preserve">J2, </t>
   </si>
   <si>
@@ -361,9 +358,6 @@
     <t>Custom, Done</t>
   </si>
   <si>
-    <t>UJ2-MBH-1-SMT-TR</t>
-  </si>
-  <si>
     <t>PJ-102AH</t>
   </si>
   <si>
@@ -494,12 +488,18 @@
   </si>
   <si>
     <t>01x05_2.54mm</t>
+  </si>
+  <si>
+    <t>KUSBX-SL-CS1N14-B</t>
+  </si>
+  <si>
+    <t>USB_C_Recept</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1011,10 +1011,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="17" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1373,12 +1373,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,11 +1393,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F1" s="6">
         <f>SUM(G2:G50)</f>
-        <v>83.394999999999996</v>
+        <v>85.954999999999984</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1411,16 +1411,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1434,10 +1434,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3">
         <v>0.1</v>
@@ -1458,10 +1458,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="3">
         <v>0.1</v>
@@ -1482,10 +1482,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="3">
         <v>0.12</v>
@@ -1506,10 +1506,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3">
         <v>0.05</v>
@@ -1530,10 +1530,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="3">
         <v>0.38</v>
@@ -1554,10 +1554,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3">
         <v>0.1</v>
@@ -1578,10 +1578,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
         <v>98</v>
-      </c>
-      <c r="E9" t="s">
-        <v>99</v>
       </c>
       <c r="F9" s="3">
         <v>0.37</v>
@@ -1599,13 +1599,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="3">
         <v>0.19</v>
@@ -1623,13 +1623,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" s="3">
         <v>0.19</v>
@@ -1647,13 +1647,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
         <v>100</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
       </c>
       <c r="F12" s="3">
         <v>0.19</v>
@@ -1671,13 +1671,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="3">
         <v>0.45</v>
@@ -1695,13 +1695,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F14" s="3">
         <v>0.24</v>
@@ -1722,10 +1722,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F15" s="3">
         <v>0.18</v>
@@ -1743,37 +1743,37 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F16" s="3">
-        <v>0.49</v>
+        <v>3.05</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="1"/>
-        <v>0.49</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" s="3">
         <v>0.76</v>
@@ -1785,19 +1785,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F18" s="3">
         <v>0.19</v>
@@ -1809,19 +1809,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F19" s="3">
         <v>0.57999999999999996</v>
@@ -1833,19 +1833,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F20" s="3">
         <v>2.61</v>
@@ -1857,19 +1857,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="7">
         <v>734152980</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F21" s="3">
         <v>6.18</v>
@@ -1881,19 +1881,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F22" s="3">
         <v>0.86</v>
@@ -1905,19 +1905,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="1"/>
@@ -1926,19 +1926,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="1"/>
@@ -1947,19 +1947,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" s="3">
         <v>0.16</v>
@@ -1971,19 +1971,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F26" s="3">
         <v>0.1</v>
@@ -1995,19 +1995,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="3">
         <v>5.7000000000000002E-2</v>
@@ -2019,19 +2019,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" s="3">
         <v>0.1</v>
@@ -2043,19 +2043,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="3">
         <v>0.1</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -2076,10 +2076,10 @@
         <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F30" s="3">
         <v>0.1</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -2100,10 +2100,10 @@
         <v>470</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F31" s="3">
         <v>0.1</v>
@@ -2115,19 +2115,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F32" s="3">
         <v>0.1</v>
@@ -2139,19 +2139,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F33" s="3">
         <v>0.1</v>
@@ -2163,19 +2163,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="D34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F34" s="3">
         <v>0.2</v>
@@ -2187,18 +2187,18 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="9"/>
+      <c r="D35" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="G35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2206,16 +2206,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
       <c r="G36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2223,16 +2223,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
       <c r="G37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2240,19 +2240,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="F38" s="3">
         <v>0.41</v>
@@ -2264,19 +2264,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F39" s="3">
         <v>4.08</v>
@@ -2288,19 +2288,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F40" s="3">
         <v>0.55000000000000004</v>
@@ -2312,19 +2312,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F41" s="3">
         <v>0.57999999999999996</v>
@@ -2336,19 +2336,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F42" s="3">
         <v>2.81</v>
@@ -2360,19 +2360,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" s="3">
         <v>1.99</v>
@@ -2384,19 +2384,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F44" s="3">
         <v>0.33</v>
@@ -2408,19 +2408,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" t="s">
         <v>85</v>
-      </c>
-      <c r="E45" t="s">
-        <v>86</v>
       </c>
       <c r="F45" s="3">
         <v>10</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2443,19 +2443,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F47" s="3">
         <v>1.33</v>
@@ -2465,24 +2465,24 @@
         <v>1.33</v>
       </c>
       <c r="I47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F48" s="3">
         <v>21</v>
@@ -2494,19 +2494,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" t="s">
         <v>154</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="D49" t="s">
-        <v>156</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="F49" s="3">
         <v>12</v>

</xml_diff>

<commit_message>
changed regulator setup, way more board work
</commit_message>
<xml_diff>
--- a/kicad/BOM-revB.xlsx
+++ b/kicad/BOM-revB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8565D0-7917-40D5-85B8-20269F72148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA94687-47AC-4B94-9276-E16B9C655CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-revB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="157">
   <si>
     <t>Ref</t>
   </si>
@@ -223,9 +223,6 @@
     <t xml:space="preserve">U1, U5, </t>
   </si>
   <si>
-    <t>AS7805</t>
-  </si>
-  <si>
     <t xml:space="preserve">U2, </t>
   </si>
   <si>
@@ -430,9 +427,6 @@
     <t>CRCW0805470RFKEA</t>
   </si>
   <si>
-    <t>AS7805ADTR-G1</t>
-  </si>
-  <si>
     <t>TO-252-2</t>
   </si>
   <si>
@@ -494,6 +488,9 @@
   </si>
   <si>
     <t>USB_C_Recept</t>
+  </si>
+  <si>
+    <t>BD50FC0FP-E2</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1375,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,11 +1390,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="6">
         <f>SUM(G2:G50)</f>
-        <v>85.954999999999984</v>
+        <v>86.934999999999988</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1411,16 +1408,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1434,10 +1431,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" s="3">
         <v>0.1</v>
@@ -1458,10 +1455,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="3">
         <v>0.1</v>
@@ -1482,10 +1479,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="3">
         <v>0.12</v>
@@ -1506,10 +1503,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="3">
         <v>0.05</v>
@@ -1530,10 +1527,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="3">
         <v>0.38</v>
@@ -1554,10 +1551,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="3">
         <v>0.1</v>
@@ -1578,10 +1575,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
         <v>97</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
       </c>
       <c r="F9" s="3">
         <v>0.37</v>
@@ -1599,13 +1596,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F10" s="3">
         <v>0.19</v>
@@ -1623,13 +1620,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="3">
         <v>0.19</v>
@@ -1647,13 +1644,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
         <v>99</v>
-      </c>
-      <c r="E12" t="s">
-        <v>100</v>
       </c>
       <c r="F12" s="3">
         <v>0.19</v>
@@ -1671,13 +1668,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="3">
         <v>0.45</v>
@@ -1695,13 +1692,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="3">
         <v>0.24</v>
@@ -1722,10 +1719,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="3">
         <v>0.18</v>
@@ -1743,13 +1740,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="3">
         <v>3.05</v>
@@ -1770,10 +1767,10 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F17" s="3">
         <v>0.76</v>
@@ -1794,10 +1791,10 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
         <v>114</v>
-      </c>
-      <c r="E18" t="s">
-        <v>115</v>
       </c>
       <c r="F18" s="3">
         <v>0.19</v>
@@ -1818,10 +1815,10 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="F19" s="3">
         <v>0.57999999999999996</v>
@@ -1842,10 +1839,10 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="F20" s="3">
         <v>2.61</v>
@@ -1869,7 +1866,7 @@
         <v>734152980</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21" s="3">
         <v>6.18</v>
@@ -1890,10 +1887,10 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
         <v>116</v>
-      </c>
-      <c r="E22" t="s">
-        <v>117</v>
       </c>
       <c r="F22" s="3">
         <v>0.86</v>
@@ -1914,10 +1911,10 @@
         <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="1"/>
@@ -1935,10 +1932,10 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="1"/>
@@ -1956,10 +1953,10 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F25" s="3">
         <v>0.16</v>
@@ -1980,10 +1977,10 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" s="3">
         <v>0.1</v>
@@ -2004,10 +2001,10 @@
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="3">
         <v>5.7000000000000002E-2</v>
@@ -2028,10 +2025,10 @@
         <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="3">
         <v>0.1</v>
@@ -2052,10 +2049,10 @@
         <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F29" s="3">
         <v>0.1</v>
@@ -2076,10 +2073,10 @@
         <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="3">
         <v>0.1</v>
@@ -2100,10 +2097,10 @@
         <v>470</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="3">
         <v>0.1</v>
@@ -2124,10 +2121,10 @@
         <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" s="3">
         <v>0.1</v>
@@ -2148,10 +2145,10 @@
         <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="3">
         <v>0.1</v>
@@ -2172,10 +2169,10 @@
         <v>59</v>
       </c>
       <c r="D34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="F34" s="3">
         <v>0.2</v>
@@ -2196,7 +2193,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E35" s="10"/>
       <c r="G35" s="3">
@@ -2246,37 +2243,37 @@
         <v>2</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F38" s="3">
-        <v>0.41</v>
+        <v>0.9</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" si="1"/>
-        <v>0.82</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="D39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F39" s="3">
         <v>4.08</v>
@@ -2288,19 +2285,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F40" s="3">
         <v>0.55000000000000004</v>
@@ -2312,19 +2309,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F41" s="3">
         <v>0.57999999999999996</v>
@@ -2336,19 +2333,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F42" s="3">
         <v>2.81</v>
@@ -2360,19 +2357,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="3">
         <v>1.99</v>
@@ -2384,19 +2381,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F44" s="3">
         <v>0.33</v>
@@ -2408,19 +2405,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="D45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" t="s">
         <v>84</v>
-      </c>
-      <c r="E45" t="s">
-        <v>85</v>
       </c>
       <c r="F45" s="3">
         <v>10</v>
@@ -2432,7 +2429,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2443,19 +2440,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F47" s="3">
         <v>1.33</v>
@@ -2465,24 +2462,24 @@
         <v>1.33</v>
       </c>
       <c r="I47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F48" s="3">
         <v>21</v>
@@ -2494,19 +2491,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" t="s">
         <v>152</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="D49" t="s">
-        <v>154</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="F49" s="3">
         <v>12</v>

</xml_diff>